<commit_message>
creacion de funciones para ordenar
</commit_message>
<xml_diff>
--- a/RutaCritica/INGENIERÍA-CIVIL-EN-INFORMÁTICA-Y-TELECOMUNICACIONES.xlsx
+++ b/RutaCritica/INGENIERÍA-CIVIL-EN-INFORMÁTICA-Y-TELECOMUNICACIONES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Downloads\TdR\generador_de_horarios_Practica\RutaCritica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429119AF-A858-462C-BA34-4BCF0170AB92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B906A87-D50B-4E1B-86C5-D2A27877B544}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3813,8 +3813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="Q1:AB1506"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AA986" sqref="AA986:AA1007"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q1384" workbookViewId="0">
+      <selection activeCell="R1413" sqref="R1413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" outlineLevelRow="4" x14ac:dyDescent="0.2"/>

</xml_diff>